<commit_message>
Ajustes demostrativos a formatos de Solicitud gráfica
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion01/SolicitudGrafica_MA_04_01_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion01/SolicitudGrafica_MA_04_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johana Montejo Rozo\Dropbox\AULA PLANETA\Temas\Tema 1\Edición\Solicitudes Graficas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado04\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20492" windowHeight="7758" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,6 @@
     <sheet name="Definición técnica de imagenes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="176">
   <si>
     <t>Asignatura:</t>
   </si>
@@ -529,26 +528,10 @@
     <t>Ilustración</t>
   </si>
   <si>
-    <t>Conjunto de frutas</t>
-  </si>
-  <si>
-    <t>12946990
-(Ver Manuscrito Pág. 1)</t>
-  </si>
-  <si>
     <t>IMG02</t>
   </si>
   <si>
-    <t>(Ver manuscrito pág. 2)</t>
-  </si>
-  <si>
     <t>IMG03</t>
-  </si>
-  <si>
-    <t>(Ver manuscrito pág. 4)</t>
-  </si>
-  <si>
-    <t>Ilustración que representa los números pares mayores que 0 y menores que 20.</t>
   </si>
   <si>
     <t>IMG04</t>
@@ -607,6 +590,20 @@
   </si>
   <si>
     <t xml:space="preserve">Los dos conjuntos deben ir coloreados del mismo color, un color suave. </t>
+  </si>
+  <si>
+    <t>Conjunto de frutas verdes (peras, manzanas verdes, uvas verdes y limones) con la etiqueta del nombre “F” (la letra F debe ser en mayúscula). 
+La imagen del grupo de frutas verdes fue tomada de Shutterstock 12946990</t>
+  </si>
+  <si>
+    <t>12946990
+(Ver Observaciones)</t>
+  </si>
+  <si>
+    <t>(Ver Observaciones)</t>
+  </si>
+  <si>
+    <t>Conjunto de números pares del 2 al 18 representado en diagrama de Venn, es decir dentro de un círculo u óvalo con la etiqueta del nombre “P” (la letra P debe ser en mayúscula)</t>
   </si>
 </sst>
 </file>
@@ -1318,7 +1315,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1644,6 +1641,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1761,7 +1761,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropLines="16" dropStyle="combo" dx="33" fmlaLink="$K$44" fmlaRange="$K$4:$K$43" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1780,18 +1780,176 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>63833</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>3213965</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>2010723</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2053" name="Object 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2053"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>1412293</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>1335694</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2054" name="Object 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2054"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>2341055</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>1666027</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2056" name="Object 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2056"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>19150</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>9575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1038225</xdr:colOff>
+          <xdr:colOff>1038873</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>239372</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1838,15 +1996,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1047750</xdr:colOff>
+          <xdr:colOff>1048448</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>9575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>866775</xdr:colOff>
+          <xdr:colOff>866526</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>239372</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1893,15 +2051,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>19150</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>9575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>9575</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>238125</xdr:rowOff>
+          <xdr:rowOff>239372</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1950,13 +2108,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>483531</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1019724</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>713328</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2003,15 +2161,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1019175</xdr:colOff>
+          <xdr:colOff>1019724</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>483531</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>828675</xdr:colOff>
+          <xdr:colOff>828226</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>713328</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2058,15 +2216,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>9575</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>483531</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>838200</xdr:colOff>
+          <xdr:colOff>837801</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>713328</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2113,15 +2271,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>9575</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>485775</xdr:rowOff>
+          <xdr:rowOff>483531</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>838200</xdr:colOff>
+          <xdr:colOff>837801</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>714375</xdr:rowOff>
+          <xdr:rowOff>713328</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2487,16 +2645,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.2" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.875" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
@@ -2508,13 +2665,13 @@
     <col min="8" max="8" width="28.625" style="2" customWidth="1"/>
     <col min="9" max="9" width="20.5" style="2" customWidth="1"/>
     <col min="10" max="10" width="34.875" style="17" customWidth="1"/>
-    <col min="11" max="11" width="29.625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="44.25" style="17" customWidth="1"/>
     <col min="12" max="12" width="20.375" style="2" customWidth="1"/>
     <col min="13" max="13" width="14.5" style="2" customWidth="1"/>
     <col min="14" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2526,7 +2683,7 @@
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
     </row>
-    <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A2" s="1"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -2543,7 +2700,7 @@
       <c r="I2" s="55"/>
       <c r="J2" s="16"/>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>9</v>
@@ -2558,13 +2715,13 @@
       <c r="I3" s="55"/>
       <c r="J3" s="16"/>
     </row>
-    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="96" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D4" s="95"/>
       <c r="E4" s="5"/>
@@ -2579,7 +2736,7 @@
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
     </row>
-    <row r="5" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1"/>
       <c r="B5" s="6" t="s">
         <v>2</v>
@@ -2601,7 +2758,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
     </row>
-    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2614,7 +2771,7 @@
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1"/>
       <c r="B7" s="39" t="s">
         <v>41</v>
@@ -2632,7 +2789,7 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
     </row>
-    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" s="9" customFormat="1" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -2652,7 +2809,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="26.05" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="35" t="s">
         <v>3</v>
       </c>
@@ -2687,13 +2844,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="12" customFormat="1" ht="194.55" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="13" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="C10" s="27" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
@@ -2722,16 +2879,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J10" s="78" t="s">
+        <v>172</v>
+      </c>
+      <c r="K10"/>
+    </row>
+    <row r="11" spans="1:16" s="12" customFormat="1" ht="116.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="80" t="s">
         <v>151</v>
       </c>
-      <c r="K10" s="19"/>
-    </row>
-    <row r="11" spans="1:16" s="12" customFormat="1" ht="27" x14ac:dyDescent="0.25">
-      <c r="A11" s="80" t="s">
-        <v>153</v>
-      </c>
       <c r="B11" s="82" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="C11" s="27" t="str">
         <f t="shared" ref="C11:C22" si="0">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
@@ -2759,17 +2916,17 @@
         <f>IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J11" s="81" t="s">
-        <v>157</v>
-      </c>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="1:16" s="12" customFormat="1" ht="81" x14ac:dyDescent="0.25">
+      <c r="J11" s="117" t="s">
+        <v>175</v>
+      </c>
+      <c r="K11"/>
+    </row>
+    <row r="12" spans="1:16" s="12" customFormat="1" ht="139.85" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="80" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B12" s="82" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="C12" s="27" t="str">
         <f t="shared" si="0"/>
@@ -2797,17 +2954,17 @@
         <f>IF(OR(B12&lt;&gt;"",J12&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J12" s="81" t="s">
-        <v>159</v>
-      </c>
-      <c r="K12" s="19"/>
-    </row>
-    <row r="13" spans="1:16" s="12" customFormat="1" ht="40.5" x14ac:dyDescent="0.25">
+      <c r="J12" s="117" t="s">
+        <v>154</v>
+      </c>
+      <c r="K12"/>
+    </row>
+    <row r="13" spans="1:16" s="12" customFormat="1" ht="39.6" x14ac:dyDescent="0.35">
       <c r="A13" s="80" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B13" s="82" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C13" s="27" t="str">
         <f t="shared" si="0"/>
@@ -2836,16 +2993,16 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="K13" s="19"/>
     </row>
-    <row r="14" spans="1:16" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="12" customFormat="1" ht="52.8" x14ac:dyDescent="0.35">
       <c r="A14" s="80" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B14" s="82" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C14" s="27" t="str">
         <f t="shared" si="0"/>
@@ -2874,19 +3031,19 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J14" s="81" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="12" customFormat="1" ht="52.8" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="str">
         <f t="shared" ref="A15:A30" si="3">IF(OR(B15&lt;&gt;"",J15&lt;&gt;""),CONCATENATE(LEFT(A14,3),IF(MID(A14,4,2)+1&lt;10,CONCATENATE("0",MID(A14,4,2)+1))),"")</f>
         <v>IMG06</v>
       </c>
       <c r="B15" s="82" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C15" s="27" t="str">
         <f t="shared" si="0"/>
@@ -2915,18 +3072,18 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J15" s="83" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K15" s="33" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" s="12" customFormat="1" ht="52.8" x14ac:dyDescent="0.35">
       <c r="A16" s="80" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B16" s="82" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C16" s="27" t="str">
         <f t="shared" si="0"/>
@@ -2955,18 +3112,18 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J16" s="84" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="K16" s="83" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="12" customFormat="1" ht="54" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="12" customFormat="1" ht="52.8" x14ac:dyDescent="0.35">
       <c r="A17" s="80" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B17" s="82" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="C17" s="27" t="str">
         <f t="shared" si="0"/>
@@ -2995,13 +3152,13 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J17" s="84" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="K17" s="21" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3032,7 +3189,7 @@
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3063,7 +3220,7 @@
       <c r="J19" s="33"/>
       <c r="K19" s="36"/>
     </row>
-    <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3094,7 +3251,7 @@
       <c r="J20" s="19"/>
       <c r="K20" s="21"/>
     </row>
-    <row r="21" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3125,7 +3282,7 @@
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
     </row>
-    <row r="22" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3156,7 +3313,7 @@
       <c r="J22" s="14"/>
       <c r="K22" s="20"/>
     </row>
-    <row r="23" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3184,7 +3341,7 @@
       <c r="J23" s="19"/>
       <c r="K23" s="19"/>
     </row>
-    <row r="24" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3212,7 +3369,7 @@
       <c r="J24" s="14"/>
       <c r="K24" s="15"/>
     </row>
-    <row r="25" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3240,7 +3397,7 @@
       <c r="J25" s="14"/>
       <c r="K25" s="19"/>
     </row>
-    <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3268,7 +3425,7 @@
       <c r="J26" s="14"/>
       <c r="K26" s="19"/>
     </row>
-    <row r="27" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3296,7 +3453,7 @@
       <c r="J27" s="19"/>
       <c r="K27" s="19"/>
     </row>
-    <row r="28" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3324,7 +3481,7 @@
       <c r="J28" s="19"/>
       <c r="K28" s="19"/>
     </row>
-    <row r="29" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3352,7 +3509,7 @@
       <c r="J29" s="19"/>
       <c r="K29" s="19"/>
     </row>
-    <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -3380,7 +3537,7 @@
       <c r="J30" s="19"/>
       <c r="K30" s="19"/>
     </row>
-    <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="28"/>
       <c r="C31" s="28"/>
@@ -3405,7 +3562,7 @@
       <c r="J31" s="19"/>
       <c r="K31" s="19"/>
     </row>
-    <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
       <c r="B32" s="28"/>
       <c r="C32" s="28"/>
@@ -3430,7 +3587,7 @@
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
     </row>
-    <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
@@ -3455,7 +3612,7 @@
       <c r="J33" s="19"/>
       <c r="K33" s="19"/>
     </row>
-    <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="28"/>
       <c r="C34" s="28"/>
@@ -3480,7 +3637,7 @@
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
     </row>
-    <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
@@ -3505,7 +3662,7 @@
       <c r="J35" s="14"/>
       <c r="K35" s="15"/>
     </row>
-    <row r="36" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="31"/>
       <c r="C36" s="31"/>
@@ -3530,7 +3687,7 @@
       <c r="J36" s="14"/>
       <c r="K36" s="15"/>
     </row>
-    <row r="37" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
       <c r="B37" s="27"/>
       <c r="C37" s="27"/>
@@ -3555,7 +3712,7 @@
       <c r="J37" s="22"/>
       <c r="K37" s="15"/>
     </row>
-    <row r="38" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="13"/>
       <c r="B38" s="32"/>
       <c r="C38" s="32"/>
@@ -3580,7 +3737,7 @@
       <c r="J38" s="23"/>
       <c r="K38" s="15"/>
     </row>
-    <row r="39" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="27"/>
       <c r="C39" s="27"/>
@@ -3605,7 +3762,7 @@
       <c r="J39" s="14"/>
       <c r="K39" s="15"/>
     </row>
-    <row r="40" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="13"/>
       <c r="B40" s="27"/>
       <c r="C40" s="27"/>
@@ -3630,7 +3787,7 @@
       <c r="J40" s="14"/>
       <c r="K40" s="15"/>
     </row>
-    <row r="41" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="13"/>
       <c r="B41" s="27"/>
       <c r="C41" s="27"/>
@@ -3655,7 +3812,7 @@
       <c r="J41" s="14"/>
       <c r="K41" s="15"/>
     </row>
-    <row r="42" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="13"/>
       <c r="B42" s="27"/>
       <c r="C42" s="27"/>
@@ -3680,7 +3837,7 @@
       <c r="J42" s="14"/>
       <c r="K42" s="15"/>
     </row>
-    <row r="43" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="13"/>
       <c r="B43" s="27"/>
       <c r="C43" s="27"/>
@@ -3705,7 +3862,7 @@
       <c r="J43" s="14"/>
       <c r="K43" s="15"/>
     </row>
-    <row r="44" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="13"/>
       <c r="B44" s="27"/>
       <c r="C44" s="27"/>
@@ -3730,7 +3887,7 @@
       <c r="J44" s="14"/>
       <c r="K44" s="15"/>
     </row>
-    <row r="45" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="13"/>
       <c r="B45" s="27"/>
       <c r="C45" s="27"/>
@@ -3755,7 +3912,7 @@
       <c r="J45" s="14"/>
       <c r="K45" s="15"/>
     </row>
-    <row r="46" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="13"/>
       <c r="B46" s="27"/>
       <c r="C46" s="27"/>
@@ -3780,7 +3937,7 @@
       <c r="J46" s="14"/>
       <c r="K46" s="15"/>
     </row>
-    <row r="47" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="13"/>
       <c r="B47" s="27"/>
       <c r="C47" s="27"/>
@@ -3805,7 +3962,7 @@
       <c r="J47" s="14"/>
       <c r="K47" s="15"/>
     </row>
-    <row r="48" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="13"/>
       <c r="B48" s="27"/>
       <c r="C48" s="27"/>
@@ -3830,7 +3987,7 @@
       <c r="J48" s="14"/>
       <c r="K48" s="15"/>
     </row>
-    <row r="49" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="13"/>
       <c r="B49" s="27"/>
       <c r="C49" s="27"/>
@@ -3855,7 +4012,7 @@
       <c r="J49" s="14"/>
       <c r="K49" s="15"/>
     </row>
-    <row r="50" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="13"/>
       <c r="B50" s="27"/>
       <c r="C50" s="27"/>
@@ -3880,7 +4037,7 @@
       <c r="J50" s="14"/>
       <c r="K50" s="15"/>
     </row>
-    <row r="51" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="13"/>
       <c r="B51" s="27"/>
       <c r="C51" s="27"/>
@@ -3905,7 +4062,7 @@
       <c r="J51" s="14"/>
       <c r="K51" s="15"/>
     </row>
-    <row r="52" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="13"/>
       <c r="B52" s="27"/>
       <c r="C52" s="27"/>
@@ -3930,7 +4087,7 @@
       <c r="J52" s="14"/>
       <c r="K52" s="15"/>
     </row>
-    <row r="53" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="13"/>
       <c r="B53" s="27"/>
       <c r="C53" s="27"/>
@@ -3955,7 +4112,7 @@
       <c r="J53" s="14"/>
       <c r="K53" s="15"/>
     </row>
-    <row r="54" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="13"/>
       <c r="B54" s="27"/>
       <c r="C54" s="27"/>
@@ -3980,7 +4137,7 @@
       <c r="J54" s="14"/>
       <c r="K54" s="15"/>
     </row>
-    <row r="55" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="13"/>
       <c r="B55" s="27"/>
       <c r="C55" s="27"/>
@@ -4005,7 +4162,7 @@
       <c r="J55" s="14"/>
       <c r="K55" s="15"/>
     </row>
-    <row r="56" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="13"/>
       <c r="B56" s="27"/>
       <c r="C56" s="27"/>
@@ -4030,7 +4187,7 @@
       <c r="J56" s="14"/>
       <c r="K56" s="15"/>
     </row>
-    <row r="57" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="13"/>
       <c r="B57" s="27"/>
       <c r="C57" s="27"/>
@@ -4055,7 +4212,7 @@
       <c r="J57" s="14"/>
       <c r="K57" s="15"/>
     </row>
-    <row r="58" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="13"/>
       <c r="B58" s="27"/>
       <c r="C58" s="27"/>
@@ -4080,7 +4237,7 @@
       <c r="J58" s="14"/>
       <c r="K58" s="15"/>
     </row>
-    <row r="59" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="13"/>
       <c r="B59" s="27"/>
       <c r="C59" s="27"/>
@@ -4105,7 +4262,7 @@
       <c r="J59" s="14"/>
       <c r="K59" s="15"/>
     </row>
-    <row r="60" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="13"/>
       <c r="B60" s="27"/>
       <c r="C60" s="27"/>
@@ -4130,7 +4287,7 @@
       <c r="J60" s="14"/>
       <c r="K60" s="15"/>
     </row>
-    <row r="61" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="13"/>
       <c r="B61" s="27"/>
       <c r="C61" s="27"/>
@@ -4155,7 +4312,7 @@
       <c r="J61" s="14"/>
       <c r="K61" s="15"/>
     </row>
-    <row r="62" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -4180,7 +4337,7 @@
       <c r="J62" s="14"/>
       <c r="K62" s="15"/>
     </row>
-    <row r="63" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
@@ -4205,7 +4362,7 @@
       <c r="J63" s="14"/>
       <c r="K63" s="15"/>
     </row>
-    <row r="64" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
@@ -4230,7 +4387,7 @@
       <c r="J64" s="14"/>
       <c r="K64" s="15"/>
     </row>
-    <row r="65" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
@@ -4255,7 +4412,7 @@
       <c r="J65" s="14"/>
       <c r="K65" s="15"/>
     </row>
-    <row r="66" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="C66" s="13"/>
@@ -4280,7 +4437,7 @@
       <c r="J66" s="14"/>
       <c r="K66" s="15"/>
     </row>
-    <row r="67" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
@@ -4305,7 +4462,7 @@
       <c r="J67" s="14"/>
       <c r="K67" s="15"/>
     </row>
-    <row r="68" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
@@ -4330,7 +4487,7 @@
       <c r="J68" s="14"/>
       <c r="K68" s="15"/>
     </row>
-    <row r="69" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
@@ -4355,7 +4512,7 @@
       <c r="J69" s="14"/>
       <c r="K69" s="15"/>
     </row>
-    <row r="70" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13"/>
@@ -4380,7 +4537,7 @@
       <c r="J70" s="14"/>
       <c r="K70" s="15"/>
     </row>
-    <row r="71" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="13"/>
@@ -4405,7 +4562,7 @@
       <c r="J71" s="14"/>
       <c r="K71" s="15"/>
     </row>
-    <row r="72" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
@@ -4430,7 +4587,7 @@
       <c r="J72" s="14"/>
       <c r="K72" s="15"/>
     </row>
-    <row r="73" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
@@ -4455,7 +4612,7 @@
       <c r="J73" s="14"/>
       <c r="K73" s="15"/>
     </row>
-    <row r="74" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
@@ -4480,7 +4637,7 @@
       <c r="J74" s="14"/>
       <c r="K74" s="15"/>
     </row>
-    <row r="75" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
@@ -4505,7 +4662,7 @@
       <c r="J75" s="14"/>
       <c r="K75" s="15"/>
     </row>
-    <row r="76" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
@@ -4530,7 +4687,7 @@
       <c r="J76" s="14"/>
       <c r="K76" s="15"/>
     </row>
-    <row r="77" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
@@ -4555,7 +4712,7 @@
       <c r="J77" s="14"/>
       <c r="K77" s="15"/>
     </row>
-    <row r="78" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
@@ -4580,7 +4737,7 @@
       <c r="J78" s="14"/>
       <c r="K78" s="15"/>
     </row>
-    <row r="79" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
@@ -4605,7 +4762,7 @@
       <c r="J79" s="14"/>
       <c r="K79" s="15"/>
     </row>
-    <row r="80" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
@@ -4630,7 +4787,7 @@
       <c r="J80" s="14"/>
       <c r="K80" s="15"/>
     </row>
-    <row r="81" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
@@ -4655,7 +4812,7 @@
       <c r="J81" s="14"/>
       <c r="K81" s="15"/>
     </row>
-    <row r="82" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
@@ -4680,7 +4837,7 @@
       <c r="J82" s="14"/>
       <c r="K82" s="15"/>
     </row>
-    <row r="83" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
@@ -4705,7 +4862,7 @@
       <c r="J83" s="14"/>
       <c r="K83" s="15"/>
     </row>
-    <row r="84" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
@@ -4730,7 +4887,7 @@
       <c r="J84" s="14"/>
       <c r="K84" s="15"/>
     </row>
-    <row r="85" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
@@ -4755,7 +4912,7 @@
       <c r="J85" s="14"/>
       <c r="K85" s="15"/>
     </row>
-    <row r="86" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
@@ -4780,7 +4937,7 @@
       <c r="J86" s="14"/>
       <c r="K86" s="15"/>
     </row>
-    <row r="87" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="13"/>
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
@@ -4805,7 +4962,7 @@
       <c r="J87" s="14"/>
       <c r="K87" s="15"/>
     </row>
-    <row r="88" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="13"/>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -4830,7 +4987,7 @@
       <c r="J88" s="14"/>
       <c r="K88" s="15"/>
     </row>
-    <row r="89" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
@@ -4855,7 +5012,7 @@
       <c r="J89" s="14"/>
       <c r="K89" s="15"/>
     </row>
-    <row r="90" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
@@ -4880,7 +5037,7 @@
       <c r="J90" s="14"/>
       <c r="K90" s="15"/>
     </row>
-    <row r="91" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
@@ -4905,7 +5062,7 @@
       <c r="J91" s="14"/>
       <c r="K91" s="15"/>
     </row>
-    <row r="92" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
       <c r="C92" s="13"/>
@@ -4930,7 +5087,7 @@
       <c r="J92" s="14"/>
       <c r="K92" s="15"/>
     </row>
-    <row r="93" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="C93" s="13"/>
@@ -4955,7 +5112,7 @@
       <c r="J93" s="14"/>
       <c r="K93" s="15"/>
     </row>
-    <row r="94" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="C94" s="13"/>
@@ -4980,7 +5137,7 @@
       <c r="J94" s="14"/>
       <c r="K94" s="15"/>
     </row>
-    <row r="95" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="13"/>
       <c r="B95" s="13"/>
       <c r="C95" s="13"/>
@@ -5005,7 +5162,7 @@
       <c r="J95" s="14"/>
       <c r="K95" s="15"/>
     </row>
-    <row r="96" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="13"/>
       <c r="B96" s="13"/>
       <c r="C96" s="13"/>
@@ -5030,7 +5187,7 @@
       <c r="J96" s="14"/>
       <c r="K96" s="15"/>
     </row>
-    <row r="97" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="13"/>
       <c r="B97" s="13"/>
       <c r="C97" s="13"/>
@@ -5055,7 +5212,7 @@
       <c r="J97" s="14"/>
       <c r="K97" s="15"/>
     </row>
-    <row r="98" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="13"/>
       <c r="B98" s="13"/>
       <c r="C98" s="13"/>
@@ -5080,7 +5237,7 @@
       <c r="J98" s="14"/>
       <c r="K98" s="15"/>
     </row>
-    <row r="99" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="13"/>
       <c r="B99" s="13"/>
       <c r="C99" s="13"/>
@@ -5105,7 +5262,7 @@
       <c r="J99" s="14"/>
       <c r="K99" s="15"/>
     </row>
-    <row r="100" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A100" s="13"/>
       <c r="B100" s="13"/>
       <c r="C100" s="13"/>
@@ -5130,7 +5287,7 @@
       <c r="J100" s="14"/>
       <c r="K100" s="15"/>
     </row>
-    <row r="101" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A101" s="13"/>
       <c r="B101" s="13"/>
       <c r="C101" s="13"/>
@@ -5155,7 +5312,7 @@
       <c r="J101" s="14"/>
       <c r="K101" s="15"/>
     </row>
-    <row r="102" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="13"/>
       <c r="B102" s="13"/>
       <c r="C102" s="13"/>
@@ -5180,7 +5337,7 @@
       <c r="J102" s="14"/>
       <c r="K102" s="15"/>
     </row>
-    <row r="103" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="13"/>
       <c r="B103" s="13"/>
       <c r="C103" s="13"/>
@@ -5205,7 +5362,7 @@
       <c r="J103" s="14"/>
       <c r="K103" s="15"/>
     </row>
-    <row r="104" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="13"/>
       <c r="B104" s="13"/>
       <c r="C104" s="13"/>
@@ -5230,7 +5387,7 @@
       <c r="J104" s="14"/>
       <c r="K104" s="15"/>
     </row>
-    <row r="105" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A105" s="13"/>
       <c r="B105" s="13"/>
       <c r="C105" s="13"/>
@@ -5255,7 +5412,7 @@
       <c r="J105" s="14"/>
       <c r="K105" s="15"/>
     </row>
-    <row r="106" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
       <c r="C106" s="13"/>
@@ -5280,7 +5437,7 @@
       <c r="J106" s="14"/>
       <c r="K106" s="15"/>
     </row>
-    <row r="107" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="13"/>
       <c r="B107" s="13"/>
       <c r="C107" s="13"/>
@@ -5305,7 +5462,7 @@
       <c r="J107" s="14"/>
       <c r="K107" s="15"/>
     </row>
-    <row r="108" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="13"/>
       <c r="B108" s="13"/>
       <c r="C108" s="13"/>
@@ -5379,6 +5536,85 @@
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <oleObjects>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="PBrush" shapeId="2053" r:id="rId4">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>62237</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>3212369</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>2010723</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="PBrush" shapeId="2053" r:id="rId4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="PBrush" shapeId="2054" r:id="rId6">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>1412293</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>1335694</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="PBrush" shapeId="2054" r:id="rId6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="PBrush" shapeId="2056" r:id="rId8">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId9">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>2341055</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>1666027</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="PBrush" shapeId="2056" r:id="rId8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </oleObjects>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5396,7 +5632,7 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.85" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="72.25" style="37" customWidth="1"/>
     <col min="2" max="2" width="11" style="37"/>
@@ -5407,7 +5643,7 @@
     <col min="12" max="16384" width="11" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="101" t="s">
         <v>39</v>
       </c>
@@ -5417,7 +5653,7 @@
       <c r="E1" s="102"/>
       <c r="F1" s="103"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="45" t="s">
         <v>43</v>
       </c>
@@ -5429,7 +5665,7 @@
       <c r="E2" s="106"/>
       <c r="F2" s="47"/>
     </row>
-    <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
       <c r="A3" s="48" t="s">
         <v>44</v>
       </c>
@@ -5453,7 +5689,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
       <c r="A4" s="45" t="s">
         <v>45</v>
       </c>
@@ -5481,7 +5717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="79.55" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="48" t="s">
         <v>46</v>
       </c>
@@ -5508,7 +5744,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="32.049999999999997" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="45" t="s">
         <v>11</v>
       </c>
@@ -5530,7 +5766,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="32.049999999999997" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="48" t="s">
         <v>12</v>
       </c>
@@ -5557,7 +5793,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="47.5" x14ac:dyDescent="0.5">
       <c r="A8" s="48" t="s">
         <v>54</v>
       </c>
@@ -5576,7 +5812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="47.5" x14ac:dyDescent="0.5">
       <c r="A9" s="48" t="s">
         <v>13</v>
       </c>
@@ -5595,7 +5831,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="32.049999999999997" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="49" t="s">
         <v>37</v>
       </c>
@@ -5614,7 +5850,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
       <c r="I11" s="37" t="s">
         <v>33</v>
       </c>
@@ -5625,7 +5861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="I12" s="37" t="s">
         <v>38</v>
       </c>
@@ -5636,7 +5872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A13" s="101" t="s">
         <v>42</v>
       </c>
@@ -5655,7 +5891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="16.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="48"/>
       <c r="B14" s="46"/>
       <c r="C14" s="46"/>
@@ -5672,7 +5908,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A15" s="45" t="s">
         <v>47</v>
       </c>
@@ -5690,7 +5926,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="67.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="67.2" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A16" s="48" t="s">
         <v>48</v>
       </c>
@@ -5714,7 +5950,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="32.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="45" t="s">
         <v>45</v>
       </c>
@@ -5735,7 +5971,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="79.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="79.55" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="48" t="s">
         <v>49</v>
       </c>
@@ -5756,7 +5992,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A19" s="45" t="s">
         <v>11</v>
       </c>
@@ -5775,7 +6011,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="49" t="s">
         <v>52</v>
       </c>
@@ -5797,7 +6033,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="H21" s="37" t="str">
         <f>IF(INDEX(H4:H7,H20)=H4,"MA",IF(INDEX(H4:H7,H20)=H5,"CN",IF(INDEX(H4:H7,H20)=H6,"CS",IF(INDEX(H4:H7,H20)=H7,"LE"))))</f>
         <v>LE</v>
@@ -5814,122 +6050,122 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K22" s="37">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K23" s="37">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K24" s="37">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K25" s="37">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K26" s="37">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K27" s="37">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K28" s="37">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K29" s="37">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K30" s="37">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K31" s="37">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.5">
       <c r="K32" s="37">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K33" s="37">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K34" s="37">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K35" s="37">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K36" s="37">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K37" s="37">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K38" s="37">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K39" s="37">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K40" s="37">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K41" s="37">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K42" s="37">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K43" s="37">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K44" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="11:11" x14ac:dyDescent="0.5">
       <c r="K45" s="37" t="str">
         <f>CONCATENATE("REC",K44,0)</f>
         <v>REC10</v>
@@ -5963,13 +6199,13 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>483531</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1019724</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>713328</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5983,15 +6219,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1019175</xdr:colOff>
+                    <xdr:colOff>1019724</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>483531</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>828675</xdr:colOff>
+                    <xdr:colOff>828226</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>713328</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6005,15 +6241,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>9575</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>483531</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>838200</xdr:colOff>
+                    <xdr:colOff>837801</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>713328</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6027,15 +6263,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>9575</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>485775</xdr:rowOff>
+                    <xdr:rowOff>483531</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>838200</xdr:colOff>
+                    <xdr:colOff>837801</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>714375</xdr:rowOff>
+                    <xdr:rowOff>713328</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6049,15 +6285,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>19150</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>9575</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1038225</xdr:colOff>
+                    <xdr:colOff>1038873</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>239372</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6071,15 +6307,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>1047750</xdr:colOff>
+                    <xdr:colOff>1048448</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>9575</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>866775</xdr:colOff>
+                    <xdr:colOff>866526</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>239372</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6093,15 +6329,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>19150</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>9575</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>9525</xdr:colOff>
+                    <xdr:colOff>9575</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>238125</xdr:rowOff>
+                    <xdr:rowOff>239372</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6123,7 +6359,7 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.85" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="21" style="37" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="37" customWidth="1"/>
@@ -6138,7 +6374,7 @@
     <col min="12" max="16384" width="10.875" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A1" s="115" t="s">
         <v>57</v>
       </c>
@@ -6166,7 +6402,7 @@
       <c r="I1" s="116"/>
       <c r="J1" s="116"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" s="115"/>
       <c r="B2" s="115"/>
       <c r="C2" s="115"/>
@@ -6184,7 +6420,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A3" s="57" t="s">
         <v>70</v>
       </c>
@@ -6208,7 +6444,7 @@
       <c r="I3" s="57"/>
       <c r="J3" s="57"/>
     </row>
-    <row r="4" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A4" s="59" t="s">
         <v>58</v>
       </c>
@@ -6236,7 +6472,7 @@
       </c>
       <c r="J4" s="59"/>
     </row>
-    <row r="5" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A5" s="60" t="s">
         <v>81</v>
       </c>
@@ -6264,7 +6500,7 @@
       </c>
       <c r="J5" s="61"/>
     </row>
-    <row r="6" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A6" s="59" t="s">
         <v>59</v>
       </c>
@@ -6296,7 +6532,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="58" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="58" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
       <c r="A7" s="59" t="s">
         <v>85</v>
       </c>
@@ -6324,7 +6560,7 @@
       </c>
       <c r="J7" s="59"/>
     </row>
-    <row r="8" spans="1:11" s="58" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="59" t="s">
         <v>87</v>
       </c>
@@ -6352,7 +6588,7 @@
       </c>
       <c r="J8" s="59"/>
     </row>
-    <row r="9" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A9" s="59" t="s">
         <v>89</v>
       </c>
@@ -6380,7 +6616,7 @@
       </c>
       <c r="J9" s="59"/>
     </row>
-    <row r="10" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A10" s="59" t="s">
         <v>91</v>
       </c>
@@ -6404,7 +6640,7 @@
       <c r="I10" s="59"/>
       <c r="J10" s="59"/>
     </row>
-    <row r="11" spans="1:11" s="58" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="58" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
       <c r="A11" s="59" t="s">
         <v>94</v>
       </c>
@@ -6432,7 +6668,7 @@
       </c>
       <c r="J11" s="59"/>
     </row>
-    <row r="12" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="58" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A12" s="59" t="s">
         <v>96</v>
       </c>
@@ -6460,7 +6696,7 @@
       </c>
       <c r="J12" s="59"/>
     </row>
-    <row r="13" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
       <c r="A13" s="62" t="s">
         <v>98</v>
       </c>
@@ -6487,7 +6723,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A14" s="62" t="s">
         <v>102</v>
       </c>
@@ -6511,7 +6747,7 @@
       </c>
       <c r="J14" s="62"/>
     </row>
-    <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
       <c r="A15" s="62" t="s">
         <v>104</v>
       </c>
@@ -6538,7 +6774,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="95" x14ac:dyDescent="0.5">
       <c r="A16" s="64" t="s">
         <v>108</v>
       </c>
@@ -6567,7 +6803,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="26.4" x14ac:dyDescent="0.5">
       <c r="A17" s="59" t="s">
         <v>113</v>
       </c>
@@ -6596,12 +6832,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20" s="68" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A21" s="69" t="s">
         <v>120</v>
       </c>
@@ -6614,7 +6850,7 @@
       <c r="D21" s="70"/>
       <c r="E21" s="70"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A22" s="72" t="s">
         <v>123</v>
       </c>
@@ -6627,7 +6863,7 @@
       <c r="D22" s="73"/>
       <c r="E22" s="73"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A23" s="72" t="s">
         <v>126</v>
       </c>
@@ -6640,7 +6876,7 @@
       <c r="D23" s="73"/>
       <c r="E23" s="73"/>
     </row>
-    <row r="24" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="31.7" x14ac:dyDescent="0.5">
       <c r="A24" s="72" t="s">
         <v>129</v>
       </c>
@@ -6653,7 +6889,7 @@
       <c r="D24" s="73"/>
       <c r="E24" s="73"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A25" s="72" t="s">
         <v>132</v>
       </c>
@@ -6666,7 +6902,7 @@
       <c r="D25" s="73"/>
       <c r="E25" s="73"/>
     </row>
-    <row r="26" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="63.35" x14ac:dyDescent="0.5">
       <c r="A26" s="72" t="s">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
MA0401: Inclusión de indicaciones de ilustración en la solicitud gráfica ppal
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado04/guion01/SolicitudGrafica_MA_04_01_CO.xlsx
+++ b/fuentes/contenidos/grado04/guion01/SolicitudGrafica_MA_04_01_CO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="171">
   <si>
     <t>Asignatura:</t>
   </si>
@@ -1520,6 +1520,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1618,15 +1627,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1766,15 +1766,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>673100</xdr:colOff>
+          <xdr:colOff>676275</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>214313</xdr:rowOff>
+          <xdr:rowOff>219075</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>3816350</xdr:colOff>
+          <xdr:colOff>3819525</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>2224088</xdr:rowOff>
+          <xdr:rowOff>2228850</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1817,13 +1817,13 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>1506538</xdr:colOff>
+          <xdr:colOff>1504950</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>2916238</xdr:colOff>
+          <xdr:colOff>2914650</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>1381125</xdr:rowOff>
         </xdr:to>
@@ -1868,15 +1868,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>1206500</xdr:colOff>
+          <xdr:colOff>1209675</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>33337</xdr:rowOff>
+          <xdr:rowOff>28575</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>3549650</xdr:colOff>
+          <xdr:colOff>3552825</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>1700212</xdr:rowOff>
+          <xdr:rowOff>1695450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1919,15 +1919,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>968377</xdr:colOff>
+          <xdr:colOff>971550</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>39687</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>3816352</xdr:colOff>
+          <xdr:colOff>3819525</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>1987550</xdr:rowOff>
+          <xdr:rowOff>1990725</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1970,15 +1970,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>1611312</xdr:colOff>
+          <xdr:colOff>1609725</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>261938</xdr:rowOff>
+          <xdr:rowOff>266700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>3201987</xdr:colOff>
+          <xdr:colOff>3200400</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>1252538</xdr:rowOff>
+          <xdr:rowOff>1257300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2021,15 +2021,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>1492250</xdr:colOff>
+          <xdr:colOff>1495425</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>150812</xdr:rowOff>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>3340100</xdr:colOff>
+          <xdr:colOff>3343275</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>1303337</xdr:rowOff>
+          <xdr:rowOff>1304925</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2072,15 +2072,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>1508125</xdr:colOff>
+          <xdr:colOff>1504950</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>55562</xdr:rowOff>
+          <xdr:rowOff>57150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>3317875</xdr:colOff>
+          <xdr:colOff>3314700</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>1169987</xdr:rowOff>
+          <xdr:rowOff>1171575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2123,15 +2123,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>1476374</xdr:colOff>
+          <xdr:colOff>1476375</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>55563</xdr:rowOff>
+          <xdr:rowOff>57150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>3286124</xdr:colOff>
+          <xdr:colOff>3286125</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>1189038</xdr:rowOff>
+          <xdr:rowOff>1190625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2174,15 +2174,15 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>150812</xdr:colOff>
+          <xdr:colOff>152400</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>55562</xdr:rowOff>
+          <xdr:rowOff>57150</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>4579937</xdr:colOff>
+          <xdr:colOff>4581525</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>1693862</xdr:rowOff>
+          <xdr:rowOff>1695450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2939,7 +2939,7 @@
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2977,14 +2977,14 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="91" t="s">
+      <c r="C2" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="92"/>
-      <c r="F2" s="84" t="s">
+      <c r="D2" s="95"/>
+      <c r="F2" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="85"/>
+      <c r="G2" s="88"/>
       <c r="H2" s="54"/>
       <c r="I2" s="54"/>
       <c r="J2" s="16"/>
@@ -2994,12 +2994,12 @@
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="93">
+      <c r="C3" s="96">
         <v>4</v>
       </c>
-      <c r="D3" s="94"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="87"/>
+      <c r="D3" s="97"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="90"/>
       <c r="H3" s="54"/>
       <c r="I3" s="54"/>
       <c r="J3" s="16"/>
@@ -3009,10 +3009,10 @@
       <c r="B4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="98" t="s">
         <v>156</v>
       </c>
-      <c r="D4" s="94"/>
+      <c r="D4" s="97"/>
       <c r="E4" s="5"/>
       <c r="F4" s="53" t="s">
         <v>56</v>
@@ -3030,10 +3030,10 @@
       <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="96" t="s">
+      <c r="C5" s="99" t="s">
         <v>149</v>
       </c>
-      <c r="D5" s="97"/>
+      <c r="D5" s="100"/>
       <c r="E5" s="5"/>
       <c r="F5" s="51" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -3084,12 +3084,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="88" t="s">
+      <c r="F8" s="91" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="89"/>
-      <c r="H8" s="89"/>
-      <c r="I8" s="90"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="93"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -3281,7 +3281,7 @@
         <f>IF(OR(B13&lt;&gt;"",J13&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J13" s="116" t="s">
+      <c r="J13" s="84" t="s">
         <v>168</v>
       </c>
       <c r="K13" s="83"/>
@@ -3319,7 +3319,7 @@
         <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J14" s="117" t="s">
+      <c r="J14" s="85" t="s">
         <v>162</v>
       </c>
       <c r="K14" s="83"/>
@@ -3450,8 +3450,12 @@
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="D18" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>146</v>
+      </c>
       <c r="F18" s="14" t="str">
         <f t="shared" si="1"/>
         <v>MA_04_01_CO_IMG09_small</v>
@@ -3468,7 +3472,7 @@
         <f>IF(OR(B18&lt;&gt;"",J18&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J18" s="118" t="s">
+      <c r="J18" s="86" t="s">
         <v>170</v>
       </c>
       <c r="K18" s="83"/>
@@ -6078,25 +6082,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="105"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="45"/>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="104"/>
-      <c r="E2" s="105"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="108"/>
       <c r="F2" s="46"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -6104,11 +6108,11 @@
         <v>44</v>
       </c>
       <c r="B3" s="45"/>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="110"/>
-      <c r="E3" s="111"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="114"/>
       <c r="F3" s="46"/>
       <c r="H3" s="36" t="s">
         <v>19</v>
@@ -6159,11 +6163,11 @@
       <c r="C5" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="112" t="str">
+      <c r="D5" s="115" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="113"/>
+      <c r="E5" s="116"/>
       <c r="F5" s="46"/>
       <c r="H5" s="36" t="s">
         <v>23</v>
@@ -6208,12 +6212,12 @@
       <c r="C7" s="76" t="s">
         <v>144</v>
       </c>
-      <c r="D7" s="98" t="str">
+      <c r="D7" s="101" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="98"/>
-      <c r="F7" s="99"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="102"/>
       <c r="H7" s="36" t="s">
         <v>25</v>
       </c>
@@ -6307,14 +6311,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="100" t="s">
+      <c r="A13" s="103" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="101"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="102"/>
+      <c r="B13" s="104"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="104"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="105"/>
       <c r="I13" s="36" t="s">
         <v>34</v>
       </c>
@@ -6347,12 +6351,12 @@
         <v>47</v>
       </c>
       <c r="B15" s="45"/>
-      <c r="C15" s="103" t="s">
+      <c r="C15" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="104"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="D15" s="107"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="108"/>
       <c r="J15" s="36">
         <v>12</v>
       </c>
@@ -6392,12 +6396,12 @@
       <c r="C17" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="106" t="str">
+      <c r="D17" s="109" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="107"/>
-      <c r="F17" s="108"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="111"/>
       <c r="J17" s="36">
         <v>14</v>
       </c>
@@ -6413,12 +6417,12 @@
       <c r="C18" s="76" t="s">
         <v>145</v>
       </c>
-      <c r="D18" s="98" t="str">
+      <c r="D18" s="101" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="98"/>
-      <c r="F18" s="99"/>
+      <c r="E18" s="101"/>
+      <c r="F18" s="102"/>
       <c r="J18" s="36">
         <v>15</v>
       </c>
@@ -6809,41 +6813,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="117" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="114" t="s">
+      <c r="B1" s="117" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="114" t="s">
+      <c r="C1" s="117" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="114" t="s">
+      <c r="D1" s="117" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="114" t="s">
+      <c r="E1" s="117" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="114" t="s">
+      <c r="F1" s="117" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="114" t="s">
+      <c r="G1" s="117" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="115" t="s">
+      <c r="H1" s="118" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
+      <c r="I1" s="118"/>
+      <c r="J1" s="118"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="114"/>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
+      <c r="A2" s="117"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
       <c r="H2" s="55" t="s">
         <v>66</v>
       </c>

</xml_diff>